<commit_message>
Modified the cards and their data
</commit_message>
<xml_diff>
--- a/answer_sheet/model/data_source.xlsx
+++ b/answer_sheet/model/data_source.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="76">
   <si>
     <t>Matrícula</t>
   </si>
@@ -33,18 +33,6 @@
     <t>Escola</t>
   </si>
   <si>
-    <t>Escola Estadual António Suárez</t>
-  </si>
-  <si>
-    <t>Escola Estadual Sabina Lustosa</t>
-  </si>
-  <si>
-    <t>Escola Estadual Lorena Nazário</t>
-  </si>
-  <si>
-    <t>Escola Estadual Aníbal Fraga</t>
-  </si>
-  <si>
     <t>Adolfo Amaral</t>
   </si>
   <si>
@@ -195,13 +183,70 @@
     <t>Simão Sacramento</t>
   </si>
   <si>
-    <t>Escola Estadual Virgínia Rodovalho</t>
-  </si>
-  <si>
-    <t>Escola Estadual Vítor ou Victor Arruda</t>
-  </si>
-  <si>
-    <t>Escola Estadual Zubaida Couto</t>
+    <t>Colégio Estadual António Suárez</t>
+  </si>
+  <si>
+    <t>Colégio Estadual Sabina Lustosa</t>
+  </si>
+  <si>
+    <t>Colégio Estadual Lorena Nazário</t>
+  </si>
+  <si>
+    <t>Colégio Estadual Aníbal Fraga</t>
+  </si>
+  <si>
+    <t>Colégio Estadual Virgínia Rodovalho</t>
+  </si>
+  <si>
+    <t>Colégio Estadual Victor Arruda</t>
+  </si>
+  <si>
+    <t>Colégio Estadual Zubaida Couto</t>
+  </si>
+  <si>
+    <t>Município</t>
+  </si>
+  <si>
+    <t>Aparecida de Goiânia</t>
+  </si>
+  <si>
+    <t>Anápolis</t>
+  </si>
+  <si>
+    <t>Rio Verde</t>
+  </si>
+  <si>
+    <t>Luziânia</t>
+  </si>
+  <si>
+    <t>Águas Lindas de Goiás</t>
+  </si>
+  <si>
+    <t>Escola_Id</t>
+  </si>
+  <si>
+    <t>Turma</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Turma_serie</t>
+  </si>
+  <si>
+    <t>Turno</t>
+  </si>
+  <si>
+    <t>Matutino</t>
+  </si>
+  <si>
+    <t>Vespertino</t>
   </si>
 </sst>
 </file>
@@ -528,20 +573,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,716 +600,1482 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>98532320410</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2">
+        <v>91313341</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>63098348390</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3">
+        <v>5035439</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>47037251135</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4">
+        <v>98532963</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>40577441974</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5">
+        <v>52818654</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>70734775900</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6">
+        <v>93851379</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>54694603655</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7">
+        <v>16503772</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>75303173034</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8">
+        <v>46904536</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>20252050484</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9">
+        <v>60665937</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>27540789716</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10">
+        <v>90514236</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>35041200685</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11">
+        <v>64311812</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>16720297276</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12">
+        <v>95606680</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>40377183814</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13">
+        <v>69378403</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>32580337449</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14">
+        <v>22846259</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>27312443184</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15">
+        <v>88550081</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>35218237908</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16">
+        <v>35092175</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>89995309716</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17">
+        <v>91588943</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>90257398139</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18">
+        <v>7750362</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>67102566285</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19">
+        <v>25576301</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>56057289450</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20">
+        <v>91315403</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>59953181896</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21">
+        <v>37637462</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>59628947646</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22">
+        <v>38243339</v>
+      </c>
+      <c r="E22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>52521192910</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23">
+        <v>6843368</v>
+      </c>
+      <c r="E23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>67737941395</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24">
+        <v>8402092</v>
+      </c>
+      <c r="E24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>11811553834</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25">
+        <v>46305632</v>
+      </c>
+      <c r="E25" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>24111195926</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26">
+        <v>8989784</v>
+      </c>
+      <c r="E26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="F26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>50124092214</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27">
+        <v>88273679</v>
+      </c>
+      <c r="E27" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="F27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>69588022714</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28">
+        <v>42737301</v>
+      </c>
+      <c r="E28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>25877801096</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>3</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29">
+        <v>86607260</v>
+      </c>
+      <c r="E29" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="F29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>13823875577</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30">
+        <v>66018646</v>
+      </c>
+      <c r="E30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="F30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30">
+        <v>3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>78160531171</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31">
+        <v>98745745</v>
+      </c>
+      <c r="E31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31">
+        <v>3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>87816963208</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32">
+        <v>83373546</v>
+      </c>
+      <c r="E32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="F32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" t="s">
+        <v>69</v>
+      </c>
+      <c r="H32">
+        <v>3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>59653450140</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C33">
         <v>3</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33">
+        <v>71479004</v>
+      </c>
+      <c r="E33" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="F33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33">
+        <v>3</v>
+      </c>
+      <c r="I33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>54456326139</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C34">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>23757781</v>
+      </c>
+      <c r="E34" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="F34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" t="s">
+        <v>69</v>
+      </c>
+      <c r="H34">
+        <v>3</v>
+      </c>
+      <c r="I34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>27352290456</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C35">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>6129601</v>
+      </c>
+      <c r="E35" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="F35" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>47720386744</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>33660750</v>
+      </c>
+      <c r="E36" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="F36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>50934605105</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>66033471</v>
+      </c>
+      <c r="E37" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="F37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" t="s">
+        <v>70</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+      <c r="I37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>37288156393</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>40702302</v>
+      </c>
+      <c r="E38" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="F38" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" t="s">
+        <v>70</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+      <c r="I38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>61873154261</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>86845073</v>
+      </c>
+      <c r="E39" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="F39" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" t="s">
+        <v>69</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>69011845403</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>34103753</v>
+      </c>
+      <c r="E40" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="F40" t="s">
+        <v>66</v>
+      </c>
+      <c r="G40" t="s">
+        <v>69</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>15216670945</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C41">
-        <v>4</v>
-      </c>
-      <c r="D41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>70549655</v>
+      </c>
+      <c r="E41" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="F41" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>82668833798</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C42">
-        <v>5</v>
-      </c>
-      <c r="D42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>75980518</v>
+      </c>
+      <c r="E42" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="F42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G42" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>31867386529</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C43">
-        <v>5</v>
-      </c>
-      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>59835654</v>
+      </c>
+      <c r="E43" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="F43" t="s">
+        <v>66</v>
+      </c>
+      <c r="G43" t="s">
+        <v>70</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>99097997119</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C44">
-        <v>5</v>
-      </c>
-      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>21155946</v>
+      </c>
+      <c r="E44" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="F44" t="s">
+        <v>66</v>
+      </c>
+      <c r="G44" t="s">
+        <v>70</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>64057548260</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C45">
-        <v>5</v>
-      </c>
-      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>54715315</v>
+      </c>
+      <c r="E45" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="F45" t="s">
+        <v>66</v>
+      </c>
+      <c r="G45" t="s">
+        <v>70</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>24700375013</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C46">
-        <v>5</v>
-      </c>
-      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>71764916</v>
+      </c>
+      <c r="E46" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="F46" t="s">
+        <v>66</v>
+      </c>
+      <c r="G46" t="s">
+        <v>70</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>56493993415</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C47">
-        <v>5</v>
-      </c>
-      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>3337051</v>
+      </c>
+      <c r="E47" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="F47" t="s">
+        <v>66</v>
+      </c>
+      <c r="G47" t="s">
+        <v>70</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>29410308587</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C48">
-        <v>5</v>
-      </c>
-      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>58641961</v>
+      </c>
+      <c r="E48" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="F48" t="s">
+        <v>66</v>
+      </c>
+      <c r="G48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48" t="s">
+        <v>75</v>
+      </c>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>9543262796</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C49">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>88682372</v>
+      </c>
+      <c r="E49" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="F49" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" t="s">
+        <v>71</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>51536507682</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C50">
-        <v>5</v>
-      </c>
-      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>77171905</v>
+      </c>
+      <c r="E50" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="F50" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" t="s">
+        <v>71</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>11631776702</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C51">
-        <v>5</v>
-      </c>
-      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>46367385</v>
+      </c>
+      <c r="E51" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="F51" t="s">
+        <v>66</v>
+      </c>
+      <c r="G51" t="s">
+        <v>71</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:9">
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:9">
       <c r="B54" s="1"/>
     </row>
   </sheetData>

</xml_diff>